<commit_message>
Traceability Matrix Excel (on sheet 2)
</commit_message>
<xml_diff>
--- a/Project Documentation/Main/SDD/traceability.xlsx
+++ b/Project Documentation/Main/SDD/traceability.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="9555" windowHeight="6720"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="9555" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="60">
   <si>
     <t>SDD</t>
   </si>
@@ -136,13 +136,73 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>SAS</t>
+  </si>
+  <si>
+    <t>4.10</t>
+  </si>
+  <si>
+    <t>4.11</t>
+  </si>
+  <si>
+    <t>4.12</t>
+  </si>
+  <si>
+    <t>4.13.1</t>
+  </si>
+  <si>
+    <t>4.13.2</t>
+  </si>
+  <si>
+    <t>4.13.3</t>
+  </si>
+  <si>
+    <t>4.13.4</t>
+  </si>
+  <si>
+    <t>4.13.5</t>
+  </si>
+  <si>
+    <t>4.1.1.1</t>
+  </si>
+  <si>
+    <t>4.1.1.2</t>
+  </si>
+  <si>
+    <t>4.1.1.3</t>
+  </si>
+  <si>
+    <t>4.1.1.4</t>
+  </si>
+  <si>
+    <t>4.1.1.5</t>
+  </si>
+  <si>
+    <t>4.1.2.1</t>
+  </si>
+  <si>
+    <t>4.1.2.2</t>
+  </si>
+  <si>
+    <t>4.1.3.1</t>
+  </si>
+  <si>
+    <t>4.1.3.2</t>
+  </si>
+  <si>
+    <t>4.1.3.3</t>
+  </si>
+  <si>
+    <t>4.1.3.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,7 +227,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -527,11 +587,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -593,6 +662,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,12 +692,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -698,6 +788,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -732,6 +823,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -907,16 +999,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AH59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:S59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:34" ht="15.75" thickBot="1">
+    <row r="1" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="S1" s="7"/>
       <c r="U1" s="7"/>
       <c r="V1" s="7"/>
@@ -933,31 +1025,31 @@
       <c r="AG1" s="7"/>
       <c r="AH1" s="8"/>
     </row>
-    <row r="2" spans="2:34" ht="15.75" thickBot="1">
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="23" t="s">
+    <row r="2" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="25"/>
-    </row>
-    <row r="3" spans="2:34" ht="15.75" thickBot="1">
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="28"/>
+    </row>
+    <row r="3" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1007,8 +1099,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:34">
-      <c r="B4" s="20" t="s">
+    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1034,8 +1126,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:34">
-      <c r="B5" s="21"/>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B5" s="24"/>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1059,8 +1151,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:34">
-      <c r="B6" s="21"/>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B6" s="24"/>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1084,8 +1176,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="2:34">
-      <c r="B7" s="21"/>
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B7" s="24"/>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1109,8 +1201,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="2:34">
-      <c r="B8" s="21"/>
+    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B8" s="24"/>
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1134,8 +1226,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:34">
-      <c r="B9" s="21"/>
+    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B9" s="24"/>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1159,8 +1251,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:34">
-      <c r="B10" s="21"/>
+    <row r="10" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B10" s="24"/>
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1188,8 +1280,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:34">
-      <c r="B11" s="21"/>
+    <row r="11" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B11" s="24"/>
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1227,8 +1319,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:34">
-      <c r="B12" s="21"/>
+    <row r="12" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B12" s="24"/>
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1272,8 +1364,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="2:34">
-      <c r="B13" s="21"/>
+    <row r="13" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B13" s="24"/>
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1297,8 +1389,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:34">
-      <c r="B14" s="21"/>
+    <row r="14" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B14" s="24"/>
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1322,8 +1414,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:34">
-      <c r="B15" s="21"/>
+    <row r="15" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B15" s="24"/>
       <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1375,8 +1467,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:34">
-      <c r="B16" s="21"/>
+    <row r="16" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B16" s="24"/>
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1410,8 +1502,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:22">
-      <c r="B17" s="21"/>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="24"/>
       <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1445,8 +1537,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:22">
-      <c r="B18" s="21"/>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="24"/>
       <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1486,8 +1578,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="2:22">
-      <c r="B19" s="21"/>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="24"/>
       <c r="C19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1518,8 +1610,8 @@
       <c r="R19" s="13"/>
       <c r="S19" s="14"/>
     </row>
-    <row r="20" spans="2:22">
-      <c r="B20" s="21"/>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="24"/>
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1549,8 +1641,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:22">
-      <c r="B21" s="21"/>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="24"/>
       <c r="C21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1576,8 +1668,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:22">
-      <c r="B22" s="21"/>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="24"/>
       <c r="C22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1603,8 +1695,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:22">
-      <c r="B23" s="21"/>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="24"/>
       <c r="C23" s="2">
         <v>6.1</v>
       </c>
@@ -1638,8 +1730,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:22">
-      <c r="B24" s="21"/>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B24" s="24"/>
       <c r="C24" s="2">
         <v>6.2</v>
       </c>
@@ -1669,8 +1761,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:22">
-      <c r="B25" s="21"/>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="24"/>
       <c r="C25" s="2">
         <v>6.3</v>
       </c>
@@ -1704,8 +1796,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:22">
-      <c r="B26" s="21"/>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="24"/>
       <c r="C26" s="2">
         <v>6.4</v>
       </c>
@@ -1731,8 +1823,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:22">
-      <c r="B27" s="21"/>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="24"/>
       <c r="C27" s="2" t="s">
         <v>20</v>
       </c>
@@ -1760,8 +1852,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B28" s="22"/>
+    <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="25"/>
       <c r="C28" s="3">
         <v>6.5</v>
       </c>
@@ -1789,32 +1881,32 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:22" ht="15.75" thickBot="1"/>
-    <row r="33" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B33" s="26"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="23" t="s">
+    <row r="32" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="24"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="25"/>
-    </row>
-    <row r="34" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B34" s="28"/>
-      <c r="C34" s="29"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="27"/>
+      <c r="P33" s="27"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="27"/>
+      <c r="S33" s="28"/>
+    </row>
+    <row r="34" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="31"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="4" t="s">
         <v>15</v>
       </c>
@@ -1864,8 +1956,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="2:22" ht="15" customHeight="1">
-      <c r="B35" s="20" t="s">
+    <row r="35" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1897,8 +1989,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="2:22">
-      <c r="B36" s="21"/>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B36" s="24"/>
       <c r="C36" s="2" t="s">
         <v>3</v>
       </c>
@@ -1928,8 +2020,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:22">
-      <c r="B37" s="21"/>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B37" s="24"/>
       <c r="C37" s="2" t="s">
         <v>4</v>
       </c>
@@ -1959,8 +2051,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="2:22">
-      <c r="B38" s="21"/>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B38" s="24"/>
       <c r="C38" s="2" t="s">
         <v>5</v>
       </c>
@@ -1990,8 +2082,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="2:22">
-      <c r="B39" s="21"/>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B39" s="24"/>
       <c r="C39" s="2" t="s">
         <v>6</v>
       </c>
@@ -2021,8 +2113,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="2:22">
-      <c r="B40" s="21"/>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B40" s="24"/>
       <c r="C40" s="2" t="s">
         <v>7</v>
       </c>
@@ -2048,8 +2140,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:22">
-      <c r="B41" s="21"/>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B41" s="24"/>
       <c r="C41" s="2" t="s">
         <v>8</v>
       </c>
@@ -2073,8 +2165,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="2:22">
-      <c r="B42" s="21"/>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B42" s="24"/>
       <c r="C42" s="2" t="s">
         <v>9</v>
       </c>
@@ -2104,8 +2196,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="2:22">
-      <c r="B43" s="21"/>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B43" s="24"/>
       <c r="C43" s="2" t="s">
         <v>10</v>
       </c>
@@ -2149,8 +2241,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="2:22">
-      <c r="B44" s="21"/>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B44" s="24"/>
       <c r="C44" s="2" t="s">
         <v>11</v>
       </c>
@@ -2180,8 +2272,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="2:22">
-      <c r="B45" s="21"/>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B45" s="24"/>
       <c r="C45" s="2" t="s">
         <v>12</v>
       </c>
@@ -2211,8 +2303,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="2:22">
-      <c r="B46" s="21"/>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B46" s="24"/>
       <c r="C46" s="2" t="s">
         <v>13</v>
       </c>
@@ -2246,8 +2338,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="2:22">
-      <c r="B47" s="21"/>
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B47" s="24"/>
       <c r="C47" s="2" t="s">
         <v>14</v>
       </c>
@@ -2277,8 +2369,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="2:22">
-      <c r="B48" s="21"/>
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B48" s="24"/>
       <c r="C48" s="2" t="s">
         <v>15</v>
       </c>
@@ -2306,8 +2398,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="2:22">
-      <c r="B49" s="21"/>
+    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B49" s="24"/>
       <c r="C49" s="2" t="s">
         <v>16</v>
       </c>
@@ -2335,8 +2427,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="2:22">
-      <c r="B50" s="21"/>
+    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B50" s="24"/>
       <c r="C50" s="2" t="s">
         <v>24</v>
       </c>
@@ -2359,8 +2451,8 @@
       <c r="R50" s="13"/>
       <c r="S50" s="14"/>
     </row>
-    <row r="51" spans="2:22">
-      <c r="B51" s="21"/>
+    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B51" s="24"/>
       <c r="C51" s="2" t="s">
         <v>17</v>
       </c>
@@ -2384,8 +2476,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="2:22">
-      <c r="B52" s="21"/>
+    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B52" s="24"/>
       <c r="C52" s="2" t="s">
         <v>18</v>
       </c>
@@ -2409,8 +2501,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="2:22">
-      <c r="B53" s="21"/>
+    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B53" s="24"/>
       <c r="C53" s="2" t="s">
         <v>19</v>
       </c>
@@ -2434,8 +2526,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="2:22">
-      <c r="B54" s="21"/>
+    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B54" s="24"/>
       <c r="C54" s="2">
         <v>6.1</v>
       </c>
@@ -2463,8 +2555,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="2:22">
-      <c r="B55" s="21"/>
+    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B55" s="24"/>
       <c r="C55" s="2">
         <v>6.2</v>
       </c>
@@ -2490,8 +2582,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="2:22">
-      <c r="B56" s="21"/>
+    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B56" s="24"/>
       <c r="C56" s="2">
         <v>6.3</v>
       </c>
@@ -2523,8 +2615,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="2:22">
-      <c r="B57" s="21"/>
+    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B57" s="24"/>
       <c r="C57" s="2">
         <v>6.4</v>
       </c>
@@ -2554,8 +2646,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="2:22">
-      <c r="B58" s="21"/>
+    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B58" s="24"/>
       <c r="C58" s="2" t="s">
         <v>20</v>
       </c>
@@ -2585,8 +2677,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B59" s="22"/>
+    <row r="59" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="25"/>
       <c r="C59" s="3">
         <v>6.5</v>
       </c>
@@ -2629,24 +2721,911 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="28"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="34">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D2" s="35">
+        <v>4.2</v>
+      </c>
+      <c r="E2" s="35">
+        <v>4.3</v>
+      </c>
+      <c r="F2" s="35">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G2" s="35">
+        <v>4.5</v>
+      </c>
+      <c r="H2" s="35">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I2" s="35">
+        <v>4.7</v>
+      </c>
+      <c r="J2" s="35">
+        <v>4.8</v>
+      </c>
+      <c r="K2" s="35">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L2" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="11"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="14"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="14"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="14"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="14"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="14"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="14"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="14"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="14"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="14"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="14"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="14"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="14"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="14"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="14"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="14"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="14"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="14"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="14"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="14"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="14"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="14"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="14"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="14"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="14"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="14"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="14"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
+      <c r="B30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="14"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+      <c r="B31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="14"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="14"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+      <c r="B33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="14"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+      <c r="B34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="14"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="14"/>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="22"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:R1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>